<commit_message>
change model & architecture init
</commit_message>
<xml_diff>
--- a/salamantex_assignment_workjournal.xlsx
+++ b/salamantex_assignment_workjournal.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Salamantex Assignment</t>
   </si>
@@ -101,16 +101,28 @@
     <t>writing rest tests</t>
   </si>
   <si>
-    <t>0.5</t>
-  </si>
-  <si>
-    <t>0.1</t>
+    <t>Setting up database</t>
+  </si>
+  <si>
+    <t>From</t>
+  </si>
+  <si>
+    <t>To</t>
+  </si>
+  <si>
+    <t>&gt; fehler/bugs, ein kleiner fehler und suche in config aber falscher decorator</t>
+  </si>
+  <si>
+    <t>mit querybuilder ärgern (normales sql tws soviel schöner)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="h:mm"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -160,12 +172,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -175,10 +202,25 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color auto="1"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -189,16 +231,36 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -207,7 +269,201 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="15">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="medium">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="medium">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="h:mm"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="h:mm"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="medium">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="h:mm"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="h:mm"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="medium">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="medium">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="medium">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -215,6 +471,26 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A3:F25" totalsRowCount="1" headerRowDxfId="14" totalsRowDxfId="13" headerRowBorderDxfId="11" tableBorderDxfId="12" totalsRowBorderDxfId="10">
+  <autoFilter ref="A3:F24"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Task name" totalsRowDxfId="9"/>
+    <tableColumn id="2" name="Task description" totalsRowDxfId="8"/>
+    <tableColumn id="3" name="Estimated time (hrs)" totalsRowFunction="custom" dataDxfId="6" totalsRowDxfId="7">
+      <totalsRowFormula>SUM(Tabelle1[Estimated time (hrs)])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="4" name="Actual time (hrs)" totalsRowFunction="custom" dataDxfId="4" totalsRowDxfId="5">
+      <calculatedColumnFormula>(Tabelle1[[#This Row],[To]]-Tabelle1[[#This Row],[From]])</calculatedColumnFormula>
+      <totalsRowFormula>SUM(Tabelle1[Actual time (hrs)])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="5" name="From" dataDxfId="2" totalsRowDxfId="3"/>
+    <tableColumn id="6" name="To" dataDxfId="0" totalsRowDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -480,246 +756,406 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="34.83203125" customWidth="1"/>
-    <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="15.1640625" customWidth="1"/>
+    <col min="3" max="3" width="20.5" customWidth="1"/>
+    <col min="4" max="4" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+    <row r="2" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="E3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="4" t="s">
+      <c r="B4" s="4"/>
+      <c r="C4" s="10">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D4" s="10">
+        <f>(Tabelle1[[#This Row],[To]]-Tabelle1[[#This Row],[From]])</f>
+        <v>4.1666666666666741E-2</v>
+      </c>
+      <c r="E4" s="12">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="F4" s="12">
+        <v>0.89583333333333337</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="10">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D5" s="10">
+        <f>(Tabelle1[[#This Row],[To]]-Tabelle1[[#This Row],[From]])</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="E5" s="12">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="F5" s="12">
+        <v>0.95833333333333337</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="10">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D6" s="10">
+        <f>(Tabelle1[[#This Row],[To]]-Tabelle1[[#This Row],[From]])</f>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="E6" s="12">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F6" s="12">
+        <v>0.35416666666666669</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="10">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="D7" s="10">
+        <f>(Tabelle1[[#This Row],[To]]-Tabelle1[[#This Row],[From]])</f>
+        <v>6.9444444444444198E-3</v>
+      </c>
+      <c r="E7" s="12">
+        <v>0.3576388888888889</v>
+      </c>
+      <c r="F7" s="12">
+        <v>0.36458333333333331</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="4">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="4">
-        <v>1</v>
-      </c>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="B8" s="4"/>
+      <c r="C8" s="10">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D8" s="10">
+        <f>(Tabelle1[[#This Row],[To]]-Tabelle1[[#This Row],[From]])</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="E8" s="12">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="F8" s="12">
+        <v>0.39583333333333331</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="B9" s="4"/>
+      <c r="C9" s="10">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D9" s="10">
+        <f>(Tabelle1[[#This Row],[To]]-Tabelle1[[#This Row],[From]])</f>
+        <v>8.3333333333333315E-2</v>
+      </c>
+      <c r="E9" s="12">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F9" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="G9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="4">
-        <v>2</v>
-      </c>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="B10" s="4"/>
+      <c r="C10" s="10">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D10" s="10">
+        <f>(Tabelle1[[#This Row],[To]]-Tabelle1[[#This Row],[From]])</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="4">
-        <v>1</v>
-      </c>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="B11" s="4"/>
+      <c r="C11" s="10">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D11" s="10">
+        <f>(Tabelle1[[#This Row],[To]]-Tabelle1[[#This Row],[From]])</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="4">
-        <v>2</v>
-      </c>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="B12" s="4"/>
+      <c r="C12" s="10">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D12" s="10">
+        <f>(Tabelle1[[#This Row],[To]]-Tabelle1[[#This Row],[From]])</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="4">
-        <v>1</v>
-      </c>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="B13" s="4"/>
+      <c r="C13" s="10">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D13" s="10">
+        <f>(Tabelle1[[#This Row],[To]]-Tabelle1[[#This Row],[From]])</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="B14" s="4"/>
+      <c r="C14" s="10">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="D14" s="10">
+        <f>(Tabelle1[[#This Row],[To]]-Tabelle1[[#This Row],[From]])</f>
+        <v>0</v>
+      </c>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="B15" s="4"/>
+      <c r="C15" s="10">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D15" s="10">
+        <f>(Tabelle1[[#This Row],[To]]-Tabelle1[[#This Row],[From]])</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="4">
-        <v>2</v>
-      </c>
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="B16" s="4"/>
+      <c r="C16" s="10">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D16" s="10">
+        <f>(Tabelle1[[#This Row],[To]]-Tabelle1[[#This Row],[From]])</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="4">
-        <v>2</v>
-      </c>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="B17" s="4"/>
+      <c r="C17" s="10">
+        <v>6.25E-2</v>
+      </c>
+      <c r="D17" s="10">
+        <f>(Tabelle1[[#This Row],[To]]-Tabelle1[[#This Row],[From]])</f>
+        <v>0</v>
+      </c>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="4">
-        <v>2</v>
-      </c>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="B18" s="4"/>
+      <c r="C18" s="10">
+        <v>6.25E-2</v>
+      </c>
+      <c r="D18" s="10">
+        <f>(Tabelle1[[#This Row],[To]]-Tabelle1[[#This Row],[From]])</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="4">
-        <v>1</v>
-      </c>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
+      <c r="B19" s="4"/>
+      <c r="C19" s="10">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D19" s="10">
+        <f>(Tabelle1[[#This Row],[To]]-Tabelle1[[#This Row],[From]])</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10">
+        <f>(Tabelle1[[#This Row],[To]]-Tabelle1[[#This Row],[From]])</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+      <c r="B21" s="4"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10">
+        <f>(Tabelle1[[#This Row],[To]]-Tabelle1[[#This Row],[From]])</f>
+        <v>0</v>
+      </c>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="4">
-        <v>3</v>
-      </c>
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+      <c r="B22" s="4"/>
+      <c r="C22" s="10">
+        <v>6.25E-2</v>
+      </c>
+      <c r="D22" s="10">
+        <f>(Tabelle1[[#This Row],[To]]-Tabelle1[[#This Row],[From]])</f>
+        <v>0</v>
+      </c>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="4">
-        <v>1</v>
-      </c>
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
+      <c r="B23" s="4"/>
+      <c r="C23" s="10">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D23" s="10">
+        <f>(Tabelle1[[#This Row],[To]]-Tabelle1[[#This Row],[From]])</f>
+        <v>0</v>
+      </c>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+    </row>
+    <row r="24" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="4">
-        <v>3</v>
-      </c>
-      <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C24" s="5"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C25" s="5"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C26" s="6">
-        <f>SUM(C4:C23)</f>
-        <v>22</v>
-      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="10">
+        <v>6.25E-2</v>
+      </c>
+      <c r="D24" s="10">
+        <f>(Tabelle1[[#This Row],[To]]-Tabelle1[[#This Row],[From]])</f>
+        <v>0</v>
+      </c>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+    </row>
+    <row r="25" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="11">
+        <f>SUM(Tabelle1[Estimated time (hrs)])</f>
+        <v>0.93055555555555547</v>
+      </c>
+      <c r="D25" s="14">
+        <f>SUM(Tabelle1[Actual time (hrs)])</f>
+        <v>0.24652777777777785</v>
+      </c>
+      <c r="E25" s="15"/>
+      <c r="F25" s="16"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C26" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>